<commit_message>
250d minc 5 spot changed
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEEB1BF2-B244-4BEE-B797-11C51A0AB141}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAF13E5-4C8F-4D78-B826-316D0F4C0490}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="d" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="d" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1086,7 +1087,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$V$1</c15:sqref>
@@ -3911,6 +3912,491 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>671.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>638.16052631578896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>604.67105263157896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>571.18157894736805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>537.69210526315703</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>504.20263157894698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>470.71315789473601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>437.22368421052602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>403.734210526315</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>370.244736842105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>336.75526315789398</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>303.26578947368398</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>269.77631578947302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>236.28684210526299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>202.797368421052</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>169.307894736842</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>135.81842105263101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>102.328947368421</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>68.839473684210503</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$1:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>8.956062989498939</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2498257431083495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9348158277584693</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7356533564077292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5949667021603391</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4894010060405201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4065229069473197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3386044639989292</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2803515509223793</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2278697800468592</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1780853068714396</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.1283474176368795</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0762011047468798</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0187997094847399</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9522215162907903</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8708818661174398</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.7648125193408699</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6119590195456395</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3449794316292394</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.4078169344104898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B13-419B-902B-93901CAC00C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Literature</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>247.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>317.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>526.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>604.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658.66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B13-419B-902B-93901CAC00C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1176098176"/>
+        <c:axId val="1176097760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1176098176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1176097760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1176097760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1176098176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3991,6 +4477,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4508,6 +5034,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5094,6 +6136,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F8C715-5100-4D0A-A8B6-7F1D3D22458A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5401,8 +6484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5CB30-10C3-41ED-9059-520434D88C4C}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6180,6 +7263,325 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7871E86D-6023-4C89-A9C8-AAC74AB9E535}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>671.65</v>
+      </c>
+      <c r="B1">
+        <v>8956062.9894989394</v>
+      </c>
+      <c r="C1">
+        <v>118.430536553544</v>
+      </c>
+      <c r="D1">
+        <f>B1*0.000001</f>
+        <v>8.956062989498939</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>638.16052631578896</v>
+      </c>
+      <c r="B2">
+        <v>8249825.7431083499</v>
+      </c>
+      <c r="C2">
+        <v>121.98889265365899</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D20" si="0">B2*0.000001</f>
+        <v>8.2498257431083495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>604.67105263157896</v>
+      </c>
+      <c r="B3">
+        <v>7934815.8277584696</v>
+      </c>
+      <c r="C3">
+        <v>127.955380329484</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>7.9348158277584693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>571.18157894736805</v>
+      </c>
+      <c r="B4">
+        <v>7735653.3564077299</v>
+      </c>
+      <c r="C4">
+        <v>136.36198959555301</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>7.7356533564077292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>537.69210526315703</v>
+      </c>
+      <c r="B5">
+        <v>7594966.7021603398</v>
+      </c>
+      <c r="C5">
+        <v>147.09563537128301</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.5949667021603391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>504.20263157894698</v>
+      </c>
+      <c r="B6">
+        <v>7489401.00604052</v>
+      </c>
+      <c r="C6">
+        <v>159.83253397337199</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>7.4894010060405201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>470.71315789473601</v>
+      </c>
+      <c r="B7">
+        <v>7406522.9069473203</v>
+      </c>
+      <c r="C7">
+        <v>174.00838142151699</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>7.4065229069473197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>437.22368421052602</v>
+      </c>
+      <c r="B8">
+        <v>7338604.4639989296</v>
+      </c>
+      <c r="C8">
+        <v>188.86330683527899</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>7.3386044639989292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>403.734210526315</v>
+      </c>
+      <c r="B9">
+        <v>7280351.5509223798</v>
+      </c>
+      <c r="C9">
+        <v>203.562866222937</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7.2803515509223793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>370.244736842105</v>
+      </c>
+      <c r="B10">
+        <v>7227869.7800468598</v>
+      </c>
+      <c r="C10">
+        <v>217.35388261588</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>7.2278697800468592</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>336.75526315789398</v>
+      </c>
+      <c r="B11">
+        <v>7178085.3068714403</v>
+      </c>
+      <c r="C11">
+        <v>229.68937650214201</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>7.1780853068714396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>303.26578947368398</v>
+      </c>
+      <c r="B12">
+        <v>7128347.4176368797</v>
+      </c>
+      <c r="C12">
+        <v>240.292554941791</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>7.1283474176368795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>269.77631578947302</v>
+      </c>
+      <c r="B13">
+        <v>7076201.10474688</v>
+      </c>
+      <c r="C13">
+        <v>249.22113350265801</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>7.0762011047468798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>236.28684210526299</v>
+      </c>
+      <c r="B14">
+        <v>7018799.7094847402</v>
+      </c>
+      <c r="C14">
+        <v>256.630757418629</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7.0187997094847399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>202.797368421052</v>
+      </c>
+      <c r="B15">
+        <v>6952221.5162907904</v>
+      </c>
+      <c r="C15">
+        <v>262.70302073736798</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.9522215162907903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>169.307894736842</v>
+      </c>
+      <c r="B16">
+        <v>6870881.8661174402</v>
+      </c>
+      <c r="C16">
+        <v>267.70005860372299</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6.8708818661174398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>135.81842105263101</v>
+      </c>
+      <c r="B17">
+        <v>6764812.51934087</v>
+      </c>
+      <c r="C17">
+        <v>271.891339288138</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>6.7648125193408699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>102.328947368421</v>
+      </c>
+      <c r="B18">
+        <v>6611959.0195456399</v>
+      </c>
+      <c r="C18">
+        <v>275.491028804942</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>6.6119590195456395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>68.839473684210503</v>
+      </c>
+      <c r="B19">
+        <v>6344979.4316292396</v>
+      </c>
+      <c r="C19">
+        <v>278.35893933111203</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6.3449794316292394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>35.35</v>
+      </c>
+      <c r="B20">
+        <v>5407816.9344104901</v>
+      </c>
+      <c r="C20">
+        <v>268.85478192174202</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5.4078169344104898</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8403754-388F-45EC-8E75-F6F3E2570208}">
   <dimension ref="A1:H42"/>
   <sheetViews>

</xml_diff>

<commit_message>
refine near corners, error cell volume too less
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAF13E5-4C8F-4D78-B826-316D0F4C0490}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0845A9DC-2815-4CDD-A2EF-291C57D48A73}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
@@ -4242,6 +4242,80 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Well</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> separation distance, m</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4287,6 +4361,8 @@
         <c:axId val="1176097760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9"/>
+          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4304,9 +4380,78 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Pressure, MPa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -4353,6 +4498,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>

</xml_diff>

<commit_message>
T_vs_t script corrected_minc250d again error
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0845A9DC-2815-4CDD-A2EF-291C57D48A73}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE561D5F-456E-42F0-95BA-8B7DD74BED9B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6660,8 +6660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5CB30-10C3-41ED-9059-520434D88C4C}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40:O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7442,7 +7442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7871E86D-6023-4C89-A9C8-AAC74AB9E535}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refined mesh around wells, improved results fit, created diagonal distance auto calc
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE561D5F-456E-42F0-95BA-8B7DD74BED9B}"/>
+  <xr:revisionPtr revIDLastSave="332" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7815079A-A347-4836-BDD3-E1F51FECDBCA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="d" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4573,6 +4574,1356 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Literature</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>247.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>317.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>526.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>604.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658.66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B13-419B-902B-93901CAC00C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$24:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>689.42911165688304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>654.07377259755594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>618.71843353822896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>583.36309447890096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>548.00775541957398</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512.65241636024598</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>477.297077300919</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>441.94173824159202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>406.58639918226402</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>371.23106012293698</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>335.87572106361</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300.520382004282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>265.16504294495502</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>229.80970388562699</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>194.45436482630001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>159.099025766973</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>123.743686707645</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.388347648318302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>53.033008588991002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.6776695296636</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$24:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8.9489161130279893</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2427016777384097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.92772085675987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7285928505009593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5879419081476698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4824094714069096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3995597765123096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.331663634706679</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2734261810574692</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2209521492110493</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1711656132142299</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.12141487412672</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0693103564748592</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0119288856533801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9453465917348698</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.86397031855675</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.7578020868852793</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6046975540910191</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3367087402173592</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.3894697108645593</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2446-478B-8864-A00BB3DAFD3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1176098176"/>
+        <c:axId val="1176097760"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Model</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$1:$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>671.65</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>638.16052631578896</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>604.67105263157896</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>571.18157894736805</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>537.69210526315703</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>504.20263157894698</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>470.71315789473601</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>437.22368421052602</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>403.734210526315</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>370.244736842105</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>336.75526315789398</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>303.26578947368398</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>269.77631578947302</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>236.28684210526299</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>202.797368421052</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>169.307894736842</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>135.81842105263101</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>102.328947368421</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>68.839473684210503</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>35.35</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$D$1:$D$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                      <c:pt idx="0">
+                        <c:v>8.956062989498939</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8.2498257431083495</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>7.9348158277584693</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7.7356533564077292</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7.5949667021603391</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>7.4894010060405201</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7.4065229069473197</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7.3386044639989292</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>7.2803515509223793</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>7.2278697800468592</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>7.1780853068714396</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>7.1283474176368795</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>7.0762011047468798</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>7.0187997094847399</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6.9522215162907903</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>6.8708818661174398</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>6.7648125193408699</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>6.6119590195456395</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>6.3449794316292394</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>5.4078169344104898</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-5B13-419B-902B-93901CAC00C0}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1176098176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Well</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> separation distance, m</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1176097760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1176097760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Pressure, MPa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1176098176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>698.02441960995043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>678.09837277391694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>654.45634395339334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>626.75636775300586</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>594.77599598786207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>558.47401273304729</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>518.04907644261334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>473.98144572676637</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>427.04263728498495</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>378.26157898128861</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>328.84520220525894</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>280.0641439015626</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>233.12533545978124</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>189.05770474393421</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148.63276845350026</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112.3307851986855</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.350413433541718</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>52.650437233154186</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29.008408412630644</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.0823615765971706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>9.4159217496902698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6494580592500387</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2673077157349901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0014599009906497</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7981678524904501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6371519336522393</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5080289644750096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4034707764364391</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3168460102307895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2417285178509294</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1720983392552098</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.1025127954644001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0282912265821302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.9443989720725501</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.8459014535106295</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.7269265813788603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.581850311920169</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.396084476318789</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0747558162801596</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.68487560020563</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FBB7-4E76-AEBE-F190142FAC3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>247.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>317.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>526.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>604.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>658.66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FBB7-4E76-AEBE-F190142FAC3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="932609232"/>
+        <c:axId val="932610064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="932609232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="932610064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="932610064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9.5"/>
+          <c:min val="4.7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="932609232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4693,6 +6044,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5726,6 +7157,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6341,6 +8804,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F8C715-5100-4D0A-A8B6-7F1D3D22458A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{606E7934-6E57-4E77-8E33-AE30EB657C01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F2607E-29BC-4527-B781-357DBF08CC94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6660,8 +9200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5CB30-10C3-41ED-9059-520434D88C4C}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40:O51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7440,10 +9980,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7871E86D-6023-4C89-A9C8-AAC74AB9E535}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D21"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7749,6 +10289,306 @@
       <c r="D20">
         <f t="shared" si="0"/>
         <v>5.4078169344104898</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>689.42911165688304</v>
+      </c>
+      <c r="B24">
+        <v>8948916.1130279899</v>
+      </c>
+      <c r="C24">
+        <v>118.43316962211701</v>
+      </c>
+      <c r="D24">
+        <f>B24*0.000001</f>
+        <v>8.9489161130279893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>654.07377259755594</v>
+      </c>
+      <c r="B25">
+        <v>8242701.6777384104</v>
+      </c>
+      <c r="C25">
+        <v>121.99755625494601</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D43" si="1">B25*0.000001</f>
+        <v>8.2427016777384097</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>618.71843353822896</v>
+      </c>
+      <c r="B26">
+        <v>7927720.8567598704</v>
+      </c>
+      <c r="C26">
+        <v>127.973232212916</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>7.92772085675987</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>583.36309447890096</v>
+      </c>
+      <c r="B27">
+        <v>7728592.8505009599</v>
+      </c>
+      <c r="C27">
+        <v>136.39058925606099</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>7.7285928505009593</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>548.00775541957398</v>
+      </c>
+      <c r="B28">
+        <v>7587941.9081476703</v>
+      </c>
+      <c r="C28">
+        <v>147.13489559559699</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>7.5879419081476698</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>512.65241636024598</v>
+      </c>
+      <c r="B29">
+        <v>7482409.4714069096</v>
+      </c>
+      <c r="C29">
+        <v>159.88115033947699</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>7.4824094714069096</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>477.297077300919</v>
+      </c>
+      <c r="B30">
+        <v>7399559.7765123099</v>
+      </c>
+      <c r="C30">
+        <v>174.06459982605099</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>7.3995597765123096</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>441.94173824159202</v>
+      </c>
+      <c r="B31">
+        <v>7331663.6347066797</v>
+      </c>
+      <c r="C31">
+        <v>188.92549697779501</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>7.331663634706679</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>406.58639918226402</v>
+      </c>
+      <c r="B32">
+        <v>7273426.1810574699</v>
+      </c>
+      <c r="C32">
+        <v>203.629479912096</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>7.2734261810574692</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>371.23106012293698</v>
+      </c>
+      <c r="B33">
+        <v>7220952.14921105</v>
+      </c>
+      <c r="C33">
+        <v>217.42297172184999</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>7.2209521492110493</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>335.87572106361</v>
+      </c>
+      <c r="B34">
+        <v>7171165.6132142302</v>
+      </c>
+      <c r="C34">
+        <v>229.75824574157201</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>7.1711656132142299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>300.520382004282</v>
+      </c>
+      <c r="B35">
+        <v>7121414.8741267202</v>
+      </c>
+      <c r="C35">
+        <v>240.35845906387999</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>7.12141487412672</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>265.16504294495502</v>
+      </c>
+      <c r="B36">
+        <v>7069310.3564748596</v>
+      </c>
+      <c r="C36">
+        <v>249.28647916109</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>7.0693103564748592</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>229.80970388562699</v>
+      </c>
+      <c r="B37">
+        <v>7011928.8856533803</v>
+      </c>
+      <c r="C37">
+        <v>256.69106161762301</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>7.0119288856533801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>194.45436482630001</v>
+      </c>
+      <c r="B38">
+        <v>6945346.5917348703</v>
+      </c>
+      <c r="C38">
+        <v>262.75594798154299</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>6.9453465917348698</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>159.099025766973</v>
+      </c>
+      <c r="B39">
+        <v>6863970.3185567502</v>
+      </c>
+      <c r="C39">
+        <v>267.74461309465499</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>6.86397031855675</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>123.743686707645</v>
+      </c>
+      <c r="B40">
+        <v>6757802.08688528</v>
+      </c>
+      <c r="C40">
+        <v>271.92691286961701</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>6.7578020868852793</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>88.388347648318302</v>
+      </c>
+      <c r="B41">
+        <v>6604697.5540910196</v>
+      </c>
+      <c r="C41">
+        <v>275.515722050477</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>6.6046975540910191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>53.033008588991002</v>
+      </c>
+      <c r="B42">
+        <v>6336708.7402173597</v>
+      </c>
+      <c r="C42">
+        <v>278.36160691629999</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>6.3367087402173592</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>17.6776695296636</v>
+      </c>
+      <c r="B43">
+        <v>5389469.7108645597</v>
+      </c>
+      <c r="C43">
+        <v>268.638601368102</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>5.3894697108645593</v>
       </c>
     </row>
   </sheetData>
@@ -8581,4 +11421,854 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC65E012-91EC-4E31-BE29-88D2C65508E0}">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>500</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>707.10678118654755</v>
+      </c>
+      <c r="G1">
+        <f>D1</f>
+        <v>707.10678118654755</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>493.57780054</v>
+      </c>
+      <c r="B2">
+        <f>SQRT(2)*(A1-A2)</f>
+        <v>9.0823615765971706</v>
+      </c>
+      <c r="C2">
+        <f>B2+C1</f>
+        <v>9.0823615765971706</v>
+      </c>
+      <c r="D2">
+        <v>698.02441960995043</v>
+      </c>
+      <c r="E2">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F2">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G22" si="0">D2</f>
+        <v>698.02441960995043</v>
+      </c>
+      <c r="H2">
+        <f>P2*0.000001</f>
+        <v>9.4159217496902698</v>
+      </c>
+      <c r="N2">
+        <v>689.42911165688304</v>
+      </c>
+      <c r="O2">
+        <v>117.78497713470099</v>
+      </c>
+      <c r="P2">
+        <v>9415921.7496902701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>479.48795769999998</v>
+      </c>
+      <c r="B3">
+        <f>SQRT(2)*(A2-A3)</f>
+        <v>19.926046836033471</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C22" si="1">B3+C2</f>
+        <v>29.008408412630644</v>
+      </c>
+      <c r="D3">
+        <v>678.09837277391694</v>
+      </c>
+      <c r="E3">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F3">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>678.09837277391694</v>
+      </c>
+      <c r="H3">
+        <f>P3*0.000001</f>
+        <v>8.6494580592500387</v>
+      </c>
+      <c r="N3">
+        <v>654.07377259755594</v>
+      </c>
+      <c r="O3">
+        <v>119.03126537607601</v>
+      </c>
+      <c r="P3">
+        <v>8649458.05925004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>462.77051879999999</v>
+      </c>
+      <c r="B4">
+        <f>SQRT(2)*(A3-A4)</f>
+        <v>23.642028820523542</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>52.650437233154186</v>
+      </c>
+      <c r="D4">
+        <v>654.45634395339334</v>
+      </c>
+      <c r="E4">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F4">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>654.45634395339334</v>
+      </c>
+      <c r="H4">
+        <f>P4*0.000001</f>
+        <v>8.2673077157349901</v>
+      </c>
+      <c r="N4">
+        <v>618.71843353822896</v>
+      </c>
+      <c r="O4">
+        <v>121.564898204725</v>
+      </c>
+      <c r="P4">
+        <v>8267307.7157349903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>443.18367778999999</v>
+      </c>
+      <c r="B5">
+        <f>SQRT(2)*(A4-A5)</f>
+        <v>27.699976200387535</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>80.350413433541718</v>
+      </c>
+      <c r="D5">
+        <v>626.75636775300586</v>
+      </c>
+      <c r="E5">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F5">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>626.75636775300586</v>
+      </c>
+      <c r="H5">
+        <f>P5*0.000001</f>
+        <v>8.0014599009906497</v>
+      </c>
+      <c r="N5">
+        <v>583.36309447890096</v>
+      </c>
+      <c r="O5">
+        <v>126.07648997758</v>
+      </c>
+      <c r="P5">
+        <v>8001459.9009906501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>420.57014005000002</v>
+      </c>
+      <c r="B6">
+        <f>SQRT(2)*(A5-A6)</f>
+        <v>31.98037176514379</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>112.3307851986855</v>
+      </c>
+      <c r="D6">
+        <v>594.77599598786207</v>
+      </c>
+      <c r="E6">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F6">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>594.77599598786207</v>
+      </c>
+      <c r="H6">
+        <f>P6*0.000001</f>
+        <v>7.7981678524904501</v>
+      </c>
+      <c r="N6">
+        <v>548.00775541957398</v>
+      </c>
+      <c r="O6">
+        <v>133.35563826139301</v>
+      </c>
+      <c r="P6">
+        <v>7798167.8524904503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>394.90076152</v>
+      </c>
+      <c r="B7">
+        <f>SQRT(2)*(A6-A7)</f>
+        <v>36.301983254814772</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>148.63276845350026</v>
+      </c>
+      <c r="D7">
+        <v>558.47401273304729</v>
+      </c>
+      <c r="E7">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F7">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>558.47401273304729</v>
+      </c>
+      <c r="H7">
+        <f>P7*0.000001</f>
+        <v>7.6371519336522393</v>
+      </c>
+      <c r="N7">
+        <v>512.65241636024598</v>
+      </c>
+      <c r="O7">
+        <v>144.162441739576</v>
+      </c>
+      <c r="P7">
+        <v>7637151.9336522399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>366.31601494</v>
+      </c>
+      <c r="B8">
+        <f>SQRT(2)*(A7-A8)</f>
+        <v>40.424936290433948</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>189.05770474393421</v>
+      </c>
+      <c r="D8">
+        <v>518.04907644261334</v>
+      </c>
+      <c r="E8">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F8">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>518.04907644261334</v>
+      </c>
+      <c r="H8">
+        <f>P8*0.000001</f>
+        <v>7.5080289644750096</v>
+      </c>
+      <c r="N8">
+        <v>477.297077300919</v>
+      </c>
+      <c r="O8">
+        <v>158.88115722661399</v>
+      </c>
+      <c r="P8">
+        <v>7508028.9644750096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>335.15549442999998</v>
+      </c>
+      <c r="B9">
+        <f>SQRT(2)*(A8-A9)</f>
+        <v>44.067630715847031</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>233.12533545978124</v>
+      </c>
+      <c r="D9">
+        <v>473.98144572676637</v>
+      </c>
+      <c r="E9">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F9">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>473.98144572676637</v>
+      </c>
+      <c r="H9">
+        <f>P9*0.000001</f>
+        <v>7.4034707764364391</v>
+      </c>
+      <c r="N9">
+        <v>441.94173824159202</v>
+      </c>
+      <c r="O9">
+        <v>177.03312364626399</v>
+      </c>
+      <c r="P9">
+        <v>7403470.7764364397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>301.96474468000002</v>
+      </c>
+      <c r="B10">
+        <f>SQRT(2)*(A9-A10)</f>
+        <v>46.938808441781347</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>280.0641439015626</v>
+      </c>
+      <c r="D10">
+        <v>427.04263728498495</v>
+      </c>
+      <c r="E10">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F10">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>427.04263728498495</v>
+      </c>
+      <c r="H10">
+        <f>P10*0.000001</f>
+        <v>7.3168460102307895</v>
+      </c>
+      <c r="N10">
+        <v>406.58639918226402</v>
+      </c>
+      <c r="O10">
+        <v>197.000117532475</v>
+      </c>
+      <c r="P10">
+        <v>7316846.0102307899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>267.47132756000002</v>
+      </c>
+      <c r="B11">
+        <f>SQRT(2)*(A10-A11)</f>
+        <v>48.781058303696312</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>328.84520220525894</v>
+      </c>
+      <c r="D11">
+        <v>378.26157898128861</v>
+      </c>
+      <c r="E11">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F11">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>378.26157898128861</v>
+      </c>
+      <c r="H11">
+        <f>P11*0.000001</f>
+        <v>7.2417285178509294</v>
+      </c>
+      <c r="N11">
+        <v>371.23106012293698</v>
+      </c>
+      <c r="O11">
+        <v>216.425975964191</v>
+      </c>
+      <c r="P11">
+        <v>7241728.5178509299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>232.52867244000001</v>
+      </c>
+      <c r="B12">
+        <f>SQRT(2)*(A11-A12)</f>
+        <v>49.416376776029686</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>378.26157898128861</v>
+      </c>
+      <c r="D12">
+        <v>328.84520220525894</v>
+      </c>
+      <c r="E12">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F12">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>328.84520220525894</v>
+      </c>
+      <c r="H12">
+        <f>P12*0.000001</f>
+        <v>7.1720983392552098</v>
+      </c>
+      <c r="N12">
+        <v>335.87572106361</v>
+      </c>
+      <c r="O12">
+        <v>233.22203622989201</v>
+      </c>
+      <c r="P12">
+        <v>7172098.33925521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>198.03525532</v>
+      </c>
+      <c r="B13">
+        <f>SQRT(2)*(A12-A13)</f>
+        <v>48.781058303696312</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>427.04263728498495</v>
+      </c>
+      <c r="D13">
+        <v>280.0641439015626</v>
+      </c>
+      <c r="E13">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F13">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>280.0641439015626</v>
+      </c>
+      <c r="H13">
+        <f>P13*0.000001</f>
+        <v>7.1025127954644001</v>
+      </c>
+      <c r="N13">
+        <v>300.520382004282</v>
+      </c>
+      <c r="O13">
+        <v>246.445931194965</v>
+      </c>
+      <c r="P13">
+        <v>7102512.7954644002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>164.84450557</v>
+      </c>
+      <c r="B14">
+        <f>SQRT(2)*(A13-A14)</f>
+        <v>46.938808441781433</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>473.98144572676637</v>
+      </c>
+      <c r="D14">
+        <v>233.12533545978124</v>
+      </c>
+      <c r="E14">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F14">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>233.12533545978124</v>
+      </c>
+      <c r="H14">
+        <f>P14*0.000001</f>
+        <v>7.0282912265821302</v>
+      </c>
+      <c r="N14">
+        <v>265.16504294495502</v>
+      </c>
+      <c r="O14">
+        <v>256.36654520441698</v>
+      </c>
+      <c r="P14">
+        <v>7028291.2265821304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>133.68398506</v>
+      </c>
+      <c r="B15">
+        <f>SQRT(2)*(A14-A15)</f>
+        <v>44.067630715846995</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>518.04907644261334</v>
+      </c>
+      <c r="D15">
+        <v>189.05770474393421</v>
+      </c>
+      <c r="E15">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F15">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>189.05770474393421</v>
+      </c>
+      <c r="H15">
+        <f>P15*0.000001</f>
+        <v>6.9443989720725501</v>
+      </c>
+      <c r="N15">
+        <v>229.80970388562699</v>
+      </c>
+      <c r="O15">
+        <v>263.56664978401301</v>
+      </c>
+      <c r="P15">
+        <v>6944398.9720725501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>105.09923848</v>
+      </c>
+      <c r="B16">
+        <f>SQRT(2)*(A15-A16)</f>
+        <v>40.424936290433948</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>558.47401273304729</v>
+      </c>
+      <c r="D16">
+        <v>148.63276845350026</v>
+      </c>
+      <c r="E16">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F16">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>148.63276845350026</v>
+      </c>
+      <c r="H16">
+        <f>P16*0.000001</f>
+        <v>6.8459014535106295</v>
+      </c>
+      <c r="N16">
+        <v>194.45436482630001</v>
+      </c>
+      <c r="O16">
+        <v>268.79742558664998</v>
+      </c>
+      <c r="P16">
+        <v>6845901.4535106299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>79.429859949999994</v>
+      </c>
+      <c r="B17">
+        <f>SQRT(2)*(A16-A17)</f>
+        <v>36.301983254814751</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>594.77599598786207</v>
+      </c>
+      <c r="D17">
+        <v>112.3307851986855</v>
+      </c>
+      <c r="E17">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F17">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>112.3307851986855</v>
+      </c>
+      <c r="H17">
+        <f>P17*0.000001</f>
+        <v>6.7269265813788603</v>
+      </c>
+      <c r="N17">
+        <v>159.099025766973</v>
+      </c>
+      <c r="O17">
+        <v>272.68735690538699</v>
+      </c>
+      <c r="P17">
+        <v>6726926.5813788604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>56.816322210000003</v>
+      </c>
+      <c r="B18">
+        <f>SQRT(2)*(A17-A18)</f>
+        <v>31.980371765143818</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>626.75636775300586</v>
+      </c>
+      <c r="D18">
+        <v>80.350413433541718</v>
+      </c>
+      <c r="E18">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F18">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>80.350413433541718</v>
+      </c>
+      <c r="H18">
+        <f>P18*0.000001</f>
+        <v>6.581850311920169</v>
+      </c>
+      <c r="N18">
+        <v>123.743686707645</v>
+      </c>
+      <c r="O18">
+        <v>275.64602760603498</v>
+      </c>
+      <c r="P18">
+        <v>6581850.3119201697</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>37.229481200000002</v>
+      </c>
+      <c r="B19">
+        <f>SQRT(2)*(A18-A19)</f>
+        <v>27.699976200387535</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>654.45634395339334</v>
+      </c>
+      <c r="D19">
+        <v>52.650437233154186</v>
+      </c>
+      <c r="E19">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F19">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>52.650437233154186</v>
+      </c>
+      <c r="H19">
+        <f>P19*0.000001</f>
+        <v>6.396084476318789</v>
+      </c>
+      <c r="N19">
+        <v>88.388347648318302</v>
+      </c>
+      <c r="O19">
+        <v>277.76652030593499</v>
+      </c>
+      <c r="P19">
+        <v>6396084.4763187896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20.512042300000001</v>
+      </c>
+      <c r="B20">
+        <f>SQRT(2)*(A19-A20)</f>
+        <v>23.64202882052356</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>678.09837277391694</v>
+      </c>
+      <c r="D20">
+        <v>29.008408412630644</v>
+      </c>
+      <c r="E20">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F20">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>29.008408412630644</v>
+      </c>
+      <c r="H20">
+        <f>P20*0.000001</f>
+        <v>6.0747558162801596</v>
+      </c>
+      <c r="N20">
+        <v>53.033008588991002</v>
+      </c>
+      <c r="O20">
+        <v>276.35840922128699</v>
+      </c>
+      <c r="P20">
+        <v>6074755.8162801601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6.4221994599999999</v>
+      </c>
+      <c r="B21">
+        <f>SQRT(2)*(A20-A21)</f>
+        <v>19.92604683603345</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>698.02441960995043</v>
+      </c>
+      <c r="D21">
+        <v>9.0823615765971706</v>
+      </c>
+      <c r="E21">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F21">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>9.0823615765971706</v>
+      </c>
+      <c r="H21">
+        <f>P21*0.000001</f>
+        <v>4.68487560020563</v>
+      </c>
+      <c r="N21">
+        <v>17.6776695296636</v>
+      </c>
+      <c r="O21">
+        <v>259.87586819825702</v>
+      </c>
+      <c r="P21">
+        <v>4684875.6002056301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <f>SQRT(2)*(A21-A22)</f>
+        <v>9.082361576597167</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>707.10678118654755</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>17.677669529663689</v>
+      </c>
+      <c r="F22">
+        <v>35.355339059327378</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>P22*0.000001</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G22">
+    <sortCondition descending="1" ref="G1:G22"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
please check tri_250d_rd.json, valid folder, volsung, model conditions correct
</commit_message>
<xml_diff>
--- a/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
+++ b/trials/minc/minc_5_spot/plotd_project/1982-witherspoon-energy recovery by water injection-fig10-data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/minc/minc_5_spot/plotd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7815079A-A347-4836-BDD3-E1F51FECDBCA}"/>
+  <xr:revisionPtr revIDLastSave="422" documentId="8_{156D23E5-B28C-4D3D-98CC-F0B15EDA5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21081BD3-B5FD-4368-A336-40FA2D139330}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
+    <workbookView xWindow="1425" yWindow="1845" windowWidth="15375" windowHeight="7995" activeTab="5" xr2:uid="{5DD71D0A-A528-4ED7-A340-2EFFD9B464A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="d" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -146,8 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5924,6 +5928,443 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$1:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$B$1:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3929130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4335040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4525590</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4659620</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4774540</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4891440</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5030990</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5223010</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5530620</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6234970</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A831-4111-88C1-421991FA5736}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$F$1:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>671.75144212722205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601.04076400856604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.33008588990299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>459.61940777123499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>388.90872965254999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>318.19805153384402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.48737341514601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176.77669529649299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.06601717790799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.355339059315398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$C$1:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8553545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8330140</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8242201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8191883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8156313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8125724</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8094180</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8055683</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7999473</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7878338</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A831-4111-88C1-421991FA5736}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1307474064"/>
+        <c:axId val="1307478224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1307474064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307478224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1307478224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307474064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6124,6 +6565,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8189,6 +8670,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8881,6 +9878,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F2607E-29BC-4527-B781-357DBF08CC94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8F98AF9-2F5E-40BF-BA4A-0C34D30F2C01}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11427,7 +12465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC65E012-91EC-4E31-BE29-88D2C65508E0}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
@@ -11459,7 +12497,7 @@
         <v>493.57780054</v>
       </c>
       <c r="B2">
-        <f>SQRT(2)*(A1-A2)</f>
+        <f t="shared" ref="B2:B22" si="0">SQRT(2)*(A1-A2)</f>
         <v>9.0823615765971706</v>
       </c>
       <c r="C2">
@@ -11476,11 +12514,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G22" si="0">D2</f>
+        <f t="shared" ref="G2:G22" si="1">D2</f>
         <v>698.02441960995043</v>
       </c>
       <c r="H2">
-        <f>P2*0.000001</f>
+        <f t="shared" ref="H2:H22" si="2">P2*0.000001</f>
         <v>9.4159217496902698</v>
       </c>
       <c r="N2">
@@ -11498,11 +12536,11 @@
         <v>479.48795769999998</v>
       </c>
       <c r="B3">
-        <f>SQRT(2)*(A2-A3)</f>
+        <f t="shared" si="0"/>
         <v>19.926046836033471</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">B3+C2</f>
+        <f t="shared" ref="C3:C22" si="3">B3+C2</f>
         <v>29.008408412630644</v>
       </c>
       <c r="D3">
@@ -11515,11 +12553,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.09837277391694</v>
       </c>
       <c r="H3">
-        <f>P3*0.000001</f>
+        <f t="shared" si="2"/>
         <v>8.6494580592500387</v>
       </c>
       <c r="N3">
@@ -11537,11 +12575,11 @@
         <v>462.77051879999999</v>
       </c>
       <c r="B4">
-        <f>SQRT(2)*(A3-A4)</f>
+        <f t="shared" si="0"/>
         <v>23.642028820523542</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52.650437233154186</v>
       </c>
       <c r="D4">
@@ -11554,11 +12592,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>654.45634395339334</v>
       </c>
       <c r="H4">
-        <f>P4*0.000001</f>
+        <f t="shared" si="2"/>
         <v>8.2673077157349901</v>
       </c>
       <c r="N4">
@@ -11576,11 +12614,11 @@
         <v>443.18367778999999</v>
       </c>
       <c r="B5">
-        <f>SQRT(2)*(A4-A5)</f>
+        <f t="shared" si="0"/>
         <v>27.699976200387535</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>80.350413433541718</v>
       </c>
       <c r="D5">
@@ -11593,11 +12631,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>626.75636775300586</v>
       </c>
       <c r="H5">
-        <f>P5*0.000001</f>
+        <f t="shared" si="2"/>
         <v>8.0014599009906497</v>
       </c>
       <c r="N5">
@@ -11615,11 +12653,11 @@
         <v>420.57014005000002</v>
       </c>
       <c r="B6">
-        <f>SQRT(2)*(A5-A6)</f>
+        <f t="shared" si="0"/>
         <v>31.98037176514379</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>112.3307851986855</v>
       </c>
       <c r="D6">
@@ -11632,11 +12670,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>594.77599598786207</v>
       </c>
       <c r="H6">
-        <f>P6*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.7981678524904501</v>
       </c>
       <c r="N6">
@@ -11654,11 +12692,11 @@
         <v>394.90076152</v>
       </c>
       <c r="B7">
-        <f>SQRT(2)*(A6-A7)</f>
+        <f t="shared" si="0"/>
         <v>36.301983254814772</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>148.63276845350026</v>
       </c>
       <c r="D7">
@@ -11671,11 +12709,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>558.47401273304729</v>
       </c>
       <c r="H7">
-        <f>P7*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.6371519336522393</v>
       </c>
       <c r="N7">
@@ -11693,11 +12731,11 @@
         <v>366.31601494</v>
       </c>
       <c r="B8">
-        <f>SQRT(2)*(A7-A8)</f>
+        <f t="shared" si="0"/>
         <v>40.424936290433948</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>189.05770474393421</v>
       </c>
       <c r="D8">
@@ -11710,11 +12748,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>518.04907644261334</v>
       </c>
       <c r="H8">
-        <f>P8*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.5080289644750096</v>
       </c>
       <c r="N8">
@@ -11732,11 +12770,11 @@
         <v>335.15549442999998</v>
       </c>
       <c r="B9">
-        <f>SQRT(2)*(A8-A9)</f>
+        <f t="shared" si="0"/>
         <v>44.067630715847031</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>233.12533545978124</v>
       </c>
       <c r="D9">
@@ -11749,11 +12787,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>473.98144572676637</v>
       </c>
       <c r="H9">
-        <f>P9*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.4034707764364391</v>
       </c>
       <c r="N9">
@@ -11771,11 +12809,11 @@
         <v>301.96474468000002</v>
       </c>
       <c r="B10">
-        <f>SQRT(2)*(A9-A10)</f>
+        <f t="shared" si="0"/>
         <v>46.938808441781347</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>280.0641439015626</v>
       </c>
       <c r="D10">
@@ -11788,11 +12826,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>427.04263728498495</v>
       </c>
       <c r="H10">
-        <f>P10*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.3168460102307895</v>
       </c>
       <c r="N10">
@@ -11810,11 +12848,11 @@
         <v>267.47132756000002</v>
       </c>
       <c r="B11">
-        <f>SQRT(2)*(A10-A11)</f>
+        <f t="shared" si="0"/>
         <v>48.781058303696312</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>328.84520220525894</v>
       </c>
       <c r="D11">
@@ -11827,11 +12865,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>378.26157898128861</v>
       </c>
       <c r="H11">
-        <f>P11*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.2417285178509294</v>
       </c>
       <c r="N11">
@@ -11849,11 +12887,11 @@
         <v>232.52867244000001</v>
       </c>
       <c r="B12">
-        <f>SQRT(2)*(A11-A12)</f>
+        <f t="shared" si="0"/>
         <v>49.416376776029686</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>378.26157898128861</v>
       </c>
       <c r="D12">
@@ -11866,11 +12904,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>328.84520220525894</v>
       </c>
       <c r="H12">
-        <f>P12*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.1720983392552098</v>
       </c>
       <c r="N12">
@@ -11888,11 +12926,11 @@
         <v>198.03525532</v>
       </c>
       <c r="B13">
-        <f>SQRT(2)*(A12-A13)</f>
+        <f t="shared" si="0"/>
         <v>48.781058303696312</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>427.04263728498495</v>
       </c>
       <c r="D13">
@@ -11905,11 +12943,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280.0641439015626</v>
       </c>
       <c r="H13">
-        <f>P13*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.1025127954644001</v>
       </c>
       <c r="N13">
@@ -11927,11 +12965,11 @@
         <v>164.84450557</v>
       </c>
       <c r="B14">
-        <f>SQRT(2)*(A13-A14)</f>
+        <f t="shared" si="0"/>
         <v>46.938808441781433</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>473.98144572676637</v>
       </c>
       <c r="D14">
@@ -11944,11 +12982,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>233.12533545978124</v>
       </c>
       <c r="H14">
-        <f>P14*0.000001</f>
+        <f t="shared" si="2"/>
         <v>7.0282912265821302</v>
       </c>
       <c r="N14">
@@ -11966,11 +13004,11 @@
         <v>133.68398506</v>
       </c>
       <c r="B15">
-        <f>SQRT(2)*(A14-A15)</f>
+        <f t="shared" si="0"/>
         <v>44.067630715846995</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>518.04907644261334</v>
       </c>
       <c r="D15">
@@ -11983,11 +13021,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.05770474393421</v>
       </c>
       <c r="H15">
-        <f>P15*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.9443989720725501</v>
       </c>
       <c r="N15">
@@ -12005,11 +13043,11 @@
         <v>105.09923848</v>
       </c>
       <c r="B16">
-        <f>SQRT(2)*(A15-A16)</f>
+        <f t="shared" si="0"/>
         <v>40.424936290433948</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>558.47401273304729</v>
       </c>
       <c r="D16">
@@ -12022,11 +13060,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>148.63276845350026</v>
       </c>
       <c r="H16">
-        <f>P16*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.8459014535106295</v>
       </c>
       <c r="N16">
@@ -12044,11 +13082,11 @@
         <v>79.429859949999994</v>
       </c>
       <c r="B17">
-        <f>SQRT(2)*(A16-A17)</f>
+        <f t="shared" si="0"/>
         <v>36.301983254814751</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>594.77599598786207</v>
       </c>
       <c r="D17">
@@ -12061,11 +13099,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>112.3307851986855</v>
       </c>
       <c r="H17">
-        <f>P17*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.7269265813788603</v>
       </c>
       <c r="N17">
@@ -12083,11 +13121,11 @@
         <v>56.816322210000003</v>
       </c>
       <c r="B18">
-        <f>SQRT(2)*(A17-A18)</f>
+        <f t="shared" si="0"/>
         <v>31.980371765143818</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>626.75636775300586</v>
       </c>
       <c r="D18">
@@ -12100,11 +13138,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80.350413433541718</v>
       </c>
       <c r="H18">
-        <f>P18*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.581850311920169</v>
       </c>
       <c r="N18">
@@ -12122,11 +13160,11 @@
         <v>37.229481200000002</v>
       </c>
       <c r="B19">
-        <f>SQRT(2)*(A18-A19)</f>
+        <f t="shared" si="0"/>
         <v>27.699976200387535</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>654.45634395339334</v>
       </c>
       <c r="D19">
@@ -12139,11 +13177,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.650437233154186</v>
       </c>
       <c r="H19">
-        <f>P19*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.396084476318789</v>
       </c>
       <c r="N19">
@@ -12161,11 +13199,11 @@
         <v>20.512042300000001</v>
       </c>
       <c r="B20">
-        <f>SQRT(2)*(A19-A20)</f>
+        <f t="shared" si="0"/>
         <v>23.64202882052356</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>678.09837277391694</v>
       </c>
       <c r="D20">
@@ -12178,11 +13216,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.008408412630644</v>
       </c>
       <c r="H20">
-        <f>P20*0.000001</f>
+        <f t="shared" si="2"/>
         <v>6.0747558162801596</v>
       </c>
       <c r="N20">
@@ -12200,11 +13238,11 @@
         <v>6.4221994599999999</v>
       </c>
       <c r="B21">
-        <f>SQRT(2)*(A20-A21)</f>
+        <f t="shared" si="0"/>
         <v>19.92604683603345</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>698.02441960995043</v>
       </c>
       <c r="D21">
@@ -12217,11 +13255,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0823615765971706</v>
       </c>
       <c r="H21">
-        <f>P21*0.000001</f>
+        <f t="shared" si="2"/>
         <v>4.68487560020563</v>
       </c>
       <c r="N21">
@@ -12239,11 +13277,11 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <f>SQRT(2)*(A21-A22)</f>
+        <f t="shared" si="0"/>
         <v>9.082361576597167</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>707.10678118654755</v>
       </c>
       <c r="D22">
@@ -12256,11 +13294,11 @@
         <v>35.355339059327378</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22">
-        <f>P22*0.000001</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -12271,4 +13309,573 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8221985-E8E6-4DEA-BD72-520F307473ED}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>F10</f>
+        <v>35.355339059315398</v>
+      </c>
+      <c r="B1" s="1">
+        <v>3929130</v>
+      </c>
+      <c r="C1" s="1">
+        <v>8553545</v>
+      </c>
+      <c r="F1">
+        <v>671.75144212722205</v>
+      </c>
+      <c r="G1">
+        <v>8.5535452870459103</v>
+      </c>
+      <c r="H1">
+        <v>123.046618763301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>F9</f>
+        <v>106.06601717790799</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4335040</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8330140</v>
+      </c>
+      <c r="F2">
+        <v>601.04076400856604</v>
+      </c>
+      <c r="G2">
+        <v>8.3301400315699592</v>
+      </c>
+      <c r="H2">
+        <v>144.650489653535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>F8</f>
+        <v>176.77669529649299</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4525590</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8242201</v>
+      </c>
+      <c r="F3">
+        <v>530.33008588990299</v>
+      </c>
+      <c r="G3">
+        <v>8.2422011946317504</v>
+      </c>
+      <c r="H3">
+        <v>176.20130416145599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>F7</f>
+        <v>247.48737341514601</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4659620</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8191883</v>
+      </c>
+      <c r="F4">
+        <v>459.61940777123499</v>
+      </c>
+      <c r="G4">
+        <v>8.1918828886000998</v>
+      </c>
+      <c r="H4">
+        <v>209.88127581695699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>F6</f>
+        <v>318.19805153384402</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4774540</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8156313</v>
+      </c>
+      <c r="F5">
+        <v>388.90872965254999</v>
+      </c>
+      <c r="G5">
+        <v>8.1563126133250492</v>
+      </c>
+      <c r="H5">
+        <v>238.71088145204999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>F5</f>
+        <v>388.90872965254999</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4891440</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8125724</v>
+      </c>
+      <c r="F6">
+        <v>318.19805153384402</v>
+      </c>
+      <c r="G6">
+        <v>8.1257238528512197</v>
+      </c>
+      <c r="H6">
+        <v>259.76197083291498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>F4</f>
+        <v>459.61940777123499</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5030990</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8094180</v>
+      </c>
+      <c r="F7">
+        <v>247.48737341514601</v>
+      </c>
+      <c r="G7">
+        <v>8.0941804920372409</v>
+      </c>
+      <c r="H7">
+        <v>273.56585336591701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>F3</f>
+        <v>530.33008588990299</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5223010</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8055683</v>
+      </c>
+      <c r="F8">
+        <v>176.77669529649299</v>
+      </c>
+      <c r="G8">
+        <v>8.0556827180860608</v>
+      </c>
+      <c r="H8">
+        <v>281.98944909088698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>F2</f>
+        <v>601.04076400856604</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5530620</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7999473</v>
+      </c>
+      <c r="F9">
+        <v>106.06601717790799</v>
+      </c>
+      <c r="G9">
+        <v>7.9994731922590496</v>
+      </c>
+      <c r="H9">
+        <v>286.77647179297901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>F1</f>
+        <v>671.75144212722205</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6234970</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7878338</v>
+      </c>
+      <c r="F10">
+        <v>35.355339059315398</v>
+      </c>
+      <c r="G10">
+        <v>7.8783376038663899</v>
+      </c>
+      <c r="H10">
+        <v>288.966962828649</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592E7498-2295-42B0-88E9-3B9AF617FAAF}">
+  <dimension ref="A2:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>671.75144212722205</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7241950</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2*0.000001</f>
+        <v>7.2419500000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2</f>
+        <v>7.2419500000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>601.04076400856604</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6549330</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C11" si="0">B3*0.000001</f>
+        <v>6.5493299999999994</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>D2&amp;", "&amp;C3</f>
+        <v>7.24195, 6.54933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>530.33008588990299</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6262470</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2624699999999995</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" ref="D4:D11" si="1">D3&amp;", "&amp;C4</f>
+        <v>7.24195, 6.54933, 6.26247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>459.61940777123499</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6092470</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>388.90872965254999</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5970050</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9700499999999996</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>318.19805153384402</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5861570</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8615699999999995</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005, 5.86157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>247.48737341514601</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5742230</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.7422300000000002</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005, 5.86157, 5.74223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>176.77669529649299</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5578930</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5789299999999997</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005, 5.86157, 5.74223, 5.57893</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>106.06601717790799</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5305870</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3058699999999996</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005, 5.86157, 5.74223, 5.57893, 5.30587</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35.355339059315398</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3393580</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.39358</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>7.24195, 6.54933, 6.26247, 6.09247, 5.97005, 5.86157, 5.74223, 5.57893, 5.30587, 3.39358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>671.75144212722205</v>
+      </c>
+      <c r="B13" s="2">
+        <v>121.09399999999999</v>
+      </c>
+      <c r="C13" s="2">
+        <f>A13</f>
+        <v>671.75144212722205</v>
+      </c>
+      <c r="D13" s="2">
+        <f>B13</f>
+        <v>121.09399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>601.04076400856604</v>
+      </c>
+      <c r="B14" s="2">
+        <v>135.28200000000001</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f>C13&amp;", "&amp;A14</f>
+        <v>671.751442127222, 601.040764008566</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>D13&amp;", "&amp;B14</f>
+        <v>121.094, 135.282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>530.33008588990299</v>
+      </c>
+      <c r="B15" s="2">
+        <v>158.34800000000001</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" ref="C15:C22" si="2">C14&amp;", "&amp;A15</f>
+        <v>671.751442127222, 601.040764008566, 530.330085889903</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" ref="D15:D22" si="3">D14&amp;", "&amp;B15</f>
+        <v>121.094, 135.282, 158.348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>459.61940777123499</v>
+      </c>
+      <c r="B16" s="2">
+        <v>186.52099999999999</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>388.90872965254999</v>
+      </c>
+      <c r="B17" s="2">
+        <v>214.029</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>318.19805153384402</v>
+      </c>
+      <c r="B18" s="2">
+        <v>236.41200000000001</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255, 318.198051533844</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029, 236.412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>247.48737341514601</v>
+      </c>
+      <c r="B19" s="2">
+        <v>252.417</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255, 318.198051533844, 247.487373415146</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029, 236.412, 252.417</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>176.77669529649299</v>
+      </c>
+      <c r="B20" s="2">
+        <v>263.37799999999999</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255, 318.198051533844, 247.487373415146, 176.776695296493</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029, 236.412, 252.417, 263.378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>106.06601717790799</v>
+      </c>
+      <c r="B21" s="2">
+        <v>267.68</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255, 318.198051533844, 247.487373415146, 176.776695296493, 106.066017177908</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029, 236.412, 252.417, 263.378, 267.68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>35.355339059315398</v>
+      </c>
+      <c r="B22" s="2">
+        <v>240.79300000000001</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>671.751442127222, 601.040764008566, 530.330085889903, 459.619407771235, 388.90872965255, 318.198051533844, 247.487373415146, 176.776695296493, 106.066017177908, 35.3553390593154</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>121.094, 135.282, 158.348, 186.521, 214.029, 236.412, 252.417, 263.378, 267.68, 240.793</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:B22">
+    <sortCondition descending="1" ref="A13:A22"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>